<commit_message>
Big upgrades to the macro_chartist tool. Can now add trendlines of several different functions, fitted to subset of data and extrapolated for each trace.
</commit_message>
<xml_diff>
--- a/Macro_Chartist/SavedData/RESPPLLOPNWW.xlsx
+++ b/Macro_Chartist/SavedData/RESPPLLOPNWW.xlsx
@@ -456,7 +456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1105"/>
+  <dimension ref="A1:B1106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9306,6 +9306,14 @@
       </c>
       <c r="B1105" t="n">
         <v>-147.25</v>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" s="2" t="n">
+        <v>45336</v>
+      </c>
+      <c r="B1106" t="n">
+        <v>-149.508</v>
       </c>
     </row>
   </sheetData>
@@ -9354,7 +9362,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2024-02-09</t>
+          <t>2024-02-20</t>
         </is>
       </c>
     </row>
@@ -9366,7 +9374,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2024-02-09</t>
+          <t>2024-02-20</t>
         </is>
       </c>
     </row>
@@ -9402,7 +9410,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2024-02-07</t>
+          <t>2024-02-14</t>
         </is>
       </c>
     </row>
@@ -9486,7 +9494,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2024-02-08 15:34:06-06</t>
+          <t>2024-02-15 15:34:04-06</t>
         </is>
       </c>
     </row>
@@ -9497,7 +9505,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>